<commit_message>
compatibility improvement and project name correction
</commit_message>
<xml_diff>
--- a/docs/r01lib_pin_table.xlsx
+++ b/docs/r01lib_pin_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedd/Desktop/dl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedd/Desktop/dl/r01/r01lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E27794-1FB3-4D41-98E7-7C89278904C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B07028-71D6-BC45-AA38-759588EB9D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24600" yWindow="3460" windowWidth="37620" windowHeight="32540" activeTab="4" xr2:uid="{F4A4BD97-1D13-3141-8799-357F4902D58A}"/>
+    <workbookView xWindow="26760" yWindow="1140" windowWidth="28860" windowHeight="25700" activeTab="4" xr2:uid="{F4A4BD97-1D13-3141-8799-357F4902D58A}"/>
   </bookViews>
   <sheets>
     <sheet name="N947" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="327">
   <si>
     <t>FRDM-MCXN947</t>
     <phoneticPr fontId="1"/>
@@ -1153,6 +1153,46 @@
   </si>
   <si>
     <t>N236 P1_8 and P1_9 are re-assigned as VCOM pins to enable UART printf output</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRDM-MCXA156</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ARD_CS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ARD_MOSI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ARD_MISO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ARD_SCK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Short pin2 and 3 by R59 to enabling SPI on Arduino connector</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Short pin2 and 3 by R60 to enabling SPI on Arduino connector</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ARD_CS, ARD_MOSI, ARD_MISO, ARD_SCK options are added on A156</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>other pin name (4)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Arduino SPI pin names of ARD_CS, ARD_MOSI, ARD_MISO, ARD_SCK are applied to all boards</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1348,7 +1388,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1394,22 +1434,22 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1419,6 +1459,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1758,7 +1816,7 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="A3:I40"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="14"/>
@@ -1766,32 +1824,33 @@
     <col min="1" max="16384" width="13.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="10" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:10" ht="14" customHeight="1">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" ht="15">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+    </row>
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1804,137 +1863,146 @@
       <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1942,58 +2010,61 @@
         <v>16</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2001,20 +2072,21 @@
         <v>19</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -2025,21 +2097,24 @@
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="4"/>
+      <c r="J16" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -2048,19 +2123,22 @@
         <v>29</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="20"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="4"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -2069,19 +2147,22 @@
         <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="I18" s="4"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -2090,19 +2171,22 @@
         <v>33</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="17"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="4"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -2110,22 +2194,23 @@
       <c r="C20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
@@ -2133,103 +2218,109 @@
       <c r="C21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
         <v>43</v>
       </c>
@@ -2237,107 +2328,113 @@
         <v>44</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="3" t="s">
         <v>168</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="3" t="s">
@@ -2345,18 +2442,19 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="3" t="s">
@@ -2364,18 +2462,19 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F34" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="3" t="s">
@@ -2383,18 +2482,19 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="3" t="s">
@@ -2404,20 +2504,21 @@
       <c r="C36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="16" t="s">
+      <c r="G36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="3" t="s">
@@ -2427,18 +2528,19 @@
       <c r="C37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="3" t="s">
@@ -2446,18 +2548,19 @@
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="3" t="s">
@@ -2465,18 +2568,19 @@
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="3"/>
@@ -2484,63 +2588,64 @@
         <v>60</v>
       </c>
       <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="C46" s="15">
+      <c r="C46" s="18">
         <v>0</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15">
+      <c r="D46" s="18"/>
+      <c r="E46" s="18">
         <v>1</v>
       </c>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15">
+      <c r="F46" s="18"/>
+      <c r="G46" s="18">
         <v>2</v>
       </c>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15">
+      <c r="H46" s="18"/>
+      <c r="I46" s="18">
         <v>3</v>
       </c>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15">
+      <c r="J46" s="18"/>
+      <c r="K46" s="18">
         <v>4</v>
       </c>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15">
+      <c r="L46" s="18"/>
+      <c r="M46" s="18">
         <v>5</v>
       </c>
-      <c r="N46" s="15"/>
+      <c r="N46" s="18"/>
     </row>
     <row r="47" spans="1:14">
       <c r="C47" s="3" t="s">
@@ -2581,7 +2686,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="18" t="s">
         <v>175</v>
       </c>
       <c r="B48" s="3">
@@ -2625,7 +2730,7 @@
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="15"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="3">
         <f>B48+1</f>
         <v>1</v>
@@ -2668,7 +2773,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="15"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="3">
         <f t="shared" ref="B50:B79" si="0">B49+1</f>
         <v>2</v>
@@ -2711,7 +2816,7 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="15"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2754,7 +2859,7 @@
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="15"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2797,7 +2902,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="15"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2840,7 +2945,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="15"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2883,7 +2988,7 @@
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="15"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2926,7 +3031,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="15"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2965,7 +3070,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="15"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3004,7 +3109,7 @@
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="15"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3039,7 +3144,7 @@
       <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="15"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3074,7 +3179,7 @@
       <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="15"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3109,7 +3214,7 @@
       <c r="N60" s="9"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="15"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3144,7 +3249,7 @@
       <c r="N61" s="9"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="15"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3179,7 +3284,7 @@
       <c r="N62" s="9"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3214,7 +3319,7 @@
       <c r="N63" s="9"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="15"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3249,7 +3354,7 @@
       <c r="N64" s="9"/>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3284,7 +3389,7 @@
       <c r="N65" s="9"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="15"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3319,7 +3424,7 @@
       <c r="N66" s="9"/>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="15"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3354,7 +3459,7 @@
       <c r="N67" s="9"/>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="15"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3389,7 +3494,7 @@
       <c r="N68" s="9"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="15"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3424,7 +3529,7 @@
       <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="15"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3459,7 +3564,7 @@
       <c r="N70" s="9"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="15"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3494,7 +3599,7 @@
       <c r="N71" s="9"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="15"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3517,7 +3622,7 @@
       <c r="N72" s="9"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="15"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3540,7 +3645,7 @@
       <c r="N73" s="9"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="15"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3563,7 +3668,7 @@
       <c r="N74" s="9"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="15"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3586,7 +3691,7 @@
       <c r="N75" s="9"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="15"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3609,7 +3714,7 @@
       <c r="N76" s="9"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="15"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3632,7 +3737,7 @@
       <c r="N77" s="9"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="15"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3659,7 +3764,7 @@
       <c r="N78" s="9"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="15"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3686,7 +3791,7 @@
       <c r="N79" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="10">
     <mergeCell ref="A48:A79"/>
     <mergeCell ref="C45:N45"/>
     <mergeCell ref="C46:D46"/>
@@ -3695,11 +3800,8 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="M46:N46"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:J4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3711,8 +3813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF8339D-3246-D248-B338-467DAA04C626}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="14"/>
@@ -3731,19 +3833,19 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="15">
       <c r="A5" s="2" t="s">
@@ -3975,7 +4077,9 @@
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="D16" s="3" t="s">
         <v>80</v>
       </c>
@@ -3987,7 +4091,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3998,7 +4102,9 @@
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>319</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>82</v>
       </c>
@@ -4010,7 +4116,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
@@ -4019,7 +4125,9 @@
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>320</v>
+      </c>
       <c r="D18" s="3" t="s">
         <v>83</v>
       </c>
@@ -4031,7 +4139,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
@@ -4040,7 +4148,9 @@
       <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>321</v>
+      </c>
       <c r="D19" s="3" t="s">
         <v>84</v>
       </c>
@@ -4052,7 +4162,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
@@ -4074,7 +4184,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="3"/>
@@ -4097,7 +4207,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -4195,7 +4305,7 @@
       <c r="F26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="18" t="s">
         <v>27</v>
       </c>
       <c r="H26" s="3"/>
@@ -4218,7 +4328,7 @@
       <c r="F27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="15"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
@@ -4435,7 +4545,7 @@
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="18" t="s">
         <v>27</v>
       </c>
       <c r="H38" s="3"/>
@@ -4456,7 +4566,7 @@
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
@@ -4521,46 +4631,46 @@
       <c r="A46" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="C47" s="15">
+      <c r="C47" s="18">
         <v>0</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15">
+      <c r="D47" s="18"/>
+      <c r="E47" s="18">
         <v>1</v>
       </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15">
+      <c r="F47" s="18"/>
+      <c r="G47" s="18">
         <v>2</v>
       </c>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15">
+      <c r="H47" s="18"/>
+      <c r="I47" s="18">
         <v>3</v>
       </c>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15">
+      <c r="J47" s="18"/>
+      <c r="K47" s="18">
         <v>4</v>
       </c>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15">
+      <c r="L47" s="18"/>
+      <c r="M47" s="18">
         <v>5</v>
       </c>
-      <c r="N47" s="15"/>
+      <c r="N47" s="18"/>
     </row>
     <row r="48" spans="1:14">
       <c r="C48" s="3" t="s">
@@ -4601,7 +4711,7 @@
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="18" t="s">
         <v>175</v>
       </c>
       <c r="B49" s="3">
@@ -4645,7 +4755,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="15"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="3">
         <f>B49+1</f>
         <v>1</v>
@@ -4688,7 +4798,7 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="15"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="3">
         <f t="shared" ref="B51:B80" si="0">B50+1</f>
         <v>2</v>
@@ -4731,7 +4841,7 @@
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="15"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4770,7 +4880,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="15"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4809,7 +4919,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="15"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4848,7 +4958,7 @@
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="15"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4891,7 +5001,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="15"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4934,7 +5044,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="15"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4965,7 +5075,7 @@
       <c r="N57" s="9"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="15"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4996,7 +5106,7 @@
       <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="15"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5027,7 +5137,7 @@
       <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="15"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5058,7 +5168,7 @@
       <c r="N60" s="9"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="15"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5089,7 +5199,7 @@
       <c r="N61" s="9"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="15"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5120,7 +5230,7 @@
       <c r="N62" s="9"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5155,7 +5265,7 @@
       <c r="N63" s="9"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="15"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5190,7 +5300,7 @@
       <c r="N64" s="9"/>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5225,7 +5335,7 @@
       <c r="N65" s="9"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="15"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5260,7 +5370,7 @@
       <c r="N66" s="9"/>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="15"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5295,7 +5405,7 @@
       <c r="N67" s="9"/>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="15"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5326,7 +5436,7 @@
       <c r="N68" s="9"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="15"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5357,7 +5467,7 @@
       <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="15"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5388,7 +5498,7 @@
       <c r="N70" s="9"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="15"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5419,7 +5529,7 @@
       <c r="N71" s="9"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="15"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5450,7 +5560,7 @@
       <c r="N72" s="9"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="15"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5473,7 +5583,7 @@
       <c r="N73" s="9"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="15"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5496,7 +5606,7 @@
       <c r="N74" s="9"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="15"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5519,7 +5629,7 @@
       <c r="N75" s="9"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="15"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5542,7 +5652,7 @@
       <c r="N76" s="9"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="15"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5565,7 +5675,7 @@
       <c r="N77" s="9"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="15"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5588,7 +5698,7 @@
       <c r="N78" s="9"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="15"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5611,7 +5721,7 @@
       <c r="N79" s="9"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="15"/>
+      <c r="A80" s="18"/>
       <c r="B80" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5657,10 +5767,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DDC342-09CC-8E4E-BCBC-273824CBDD0A}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="A3:I41"/>
+      <selection activeCell="B21" activeCellId="3" sqref="B17 B19 B20 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="14"/>
@@ -5670,7 +5780,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -5679,19 +5789,19 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="15">
       <c r="A5" s="2" t="s">
@@ -5935,14 +6045,14 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="3"/>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>131</v>
+        <v>219</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>12</v>
@@ -5953,15 +6063,18 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>12</v>
@@ -5973,14 +6086,14 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="3"/>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>319</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>12</v>
@@ -5991,103 +6104,110 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="15" t="s">
+      <c r="E22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="3" t="s">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="3" t="s">
+      <c r="E23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>12</v>
@@ -6099,14 +6219,14 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>12</v>
@@ -6118,14 +6238,14 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>12</v>
@@ -6137,14 +6257,14 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>12</v>
@@ -6156,14 +6276,14 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" s="3" t="s">
-        <v>168</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>12</v>
@@ -6175,16 +6295,14 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>12</v>
@@ -6196,16 +6314,14 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>12</v>
@@ -6215,20 +6331,18 @@
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>12</v>
@@ -6236,22 +6350,20 @@
       <c r="F31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>12</v>
@@ -6261,18 +6373,20 @@
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="15"/>
+      <c r="I32" s="18" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>12</v>
@@ -6281,19 +6395,21 @@
         <v>12</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="15"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>12</v>
@@ -6303,16 +6419,18 @@
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>12</v>
@@ -6320,18 +6438,20 @@
       <c r="F35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>12</v>
@@ -6345,12 +6465,12 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>12</v>
@@ -6364,12 +6484,12 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>12</v>
@@ -6377,20 +6497,18 @@
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>12</v>
@@ -6398,18 +6516,18 @@
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="A40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>12</v>
@@ -6417,18 +6535,20 @@
       <c r="F40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>12</v>
@@ -6436,230 +6556,206 @@
       <c r="F41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="10" t="s">
+    <row r="42" spans="1:12">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C47" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="C46" s="15">
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="C48" s="18">
         <v>0</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15">
+      <c r="D48" s="18"/>
+      <c r="E48" s="18">
         <v>1</v>
       </c>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15">
+      <c r="F48" s="18"/>
+      <c r="G48" s="18">
         <v>2</v>
       </c>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15">
+      <c r="H48" s="18"/>
+      <c r="I48" s="18">
         <v>3</v>
       </c>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15">
+      <c r="J48" s="18"/>
+      <c r="K48" s="18">
         <v>4</v>
       </c>
-      <c r="L46" s="15"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="C47" s="3" t="s">
+      <c r="L48" s="18"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="C49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="J49" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="L47" s="3" t="s">
+      <c r="L49" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="15" t="s">
+    <row r="50" spans="1:12">
+      <c r="A50" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B50" s="3">
         <v>0</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="15"/>
-      <c r="B49" s="3">
-        <f>B48+1</f>
-        <v>1</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="15"/>
-      <c r="B50" s="3">
-        <f t="shared" ref="B50:B79" si="0">B49+1</f>
-        <v>2</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>181</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>170</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="I50" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="15"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>B50+1</f>
+        <v>1</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>170</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="I51" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="15"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+        <f t="shared" ref="B52:B81" si="0">B51+1</f>
+        <v>2</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="E52" s="3" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>126</v>
+        <v>216</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>171</v>
@@ -6667,28 +6763,32 @@
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="3" t="s">
-        <v>256</v>
+        <v>99</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="15"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="E53" s="3" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>171</v>
@@ -6696,154 +6796,158 @@
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54" s="15"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>171</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
       <c r="E54" s="3" t="s">
-        <v>196</v>
+        <v>124</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>219</v>
+        <v>126</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I54" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
       <c r="K54" s="3" t="s">
-        <v>87</v>
+        <v>256</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="15"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="3" t="s">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>73</v>
+        <v>218</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I55" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
       <c r="K55" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="15"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E56" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
+      <c r="G56" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I56" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
+      <c r="K56" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="15"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
+      <c r="G57" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I57" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
+      <c r="K57" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="15"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
       <c r="I58" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>171</v>
@@ -6852,27 +6956,23 @@
       <c r="L58" s="9"/>
     </row>
     <row r="59" spans="1:12">
-      <c r="A59" s="15"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
-      <c r="E59" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="E59" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
       <c r="I59" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>171</v>
@@ -6881,27 +6981,27 @@
       <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12">
-      <c r="A60" s="15"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>221</v>
+        <v>156</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>171</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>71</v>
+        <v>241</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>171</v>
@@ -6910,27 +7010,27 @@
       <c r="L60" s="9"/>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="15"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
-      <c r="E61" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="H61" s="9" t="s">
+      <c r="E61" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F61" s="9" t="s">
         <v>170</v>
       </c>
+      <c r="G61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I61" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>171</v>
@@ -6939,27 +7039,27 @@
       <c r="L61" s="9"/>
     </row>
     <row r="62" spans="1:12">
-      <c r="A62" s="15"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>171</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>171</v>
@@ -6968,27 +7068,27 @@
       <c r="L62" s="9"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="3" t="s">
-        <v>205</v>
+        <v>141</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>171</v>
+      <c r="G63" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>171</v>
@@ -6997,27 +7097,27 @@
       <c r="L63" s="9"/>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="15"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G64" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>171</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>246</v>
+        <v>132</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>171</v>
@@ -7026,23 +7126,27 @@
       <c r="L64" s="9"/>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I65" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>171</v>
@@ -7051,23 +7155,27 @@
       <c r="L65" s="9"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="15"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>171</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
+      <c r="G66" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I66" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>171</v>
@@ -7076,27 +7184,23 @@
       <c r="L66" s="9"/>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="15"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>171</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
       <c r="I67" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>171</v>
@@ -7105,27 +7209,23 @@
       <c r="L67" s="9"/>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="15"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>171</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
-      <c r="G68" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
       <c r="I68" s="3" t="s">
-        <v>121</v>
+        <v>248</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>171</v>
@@ -7134,13 +7234,13 @@
       <c r="L68" s="9"/>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="15"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>171</v>
@@ -7148,13 +7248,13 @@
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>171</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>171</v>
@@ -7163,23 +7263,27 @@
       <c r="L69" s="9"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="15"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>171</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
+      <c r="G70" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I70" s="3" t="s">
-        <v>251</v>
+        <v>121</v>
       </c>
       <c r="J70" s="3" t="s">
         <v>171</v>
@@ -7188,13 +7292,13 @@
       <c r="L70" s="9"/>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="15"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>171</v>
@@ -7202,55 +7306,75 @@
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
+      <c r="I71" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="15"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
+      <c r="I72" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="15"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
+      <c r="G73" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
     </row>
     <row r="74" spans="1:12">
-      <c r="A74" s="15"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
@@ -7264,10 +7388,10 @@
       <c r="L74" s="9"/>
     </row>
     <row r="75" spans="1:12">
-      <c r="A75" s="15"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
@@ -7275,20 +7399,16 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
-      <c r="I75" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="15"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
@@ -7296,33 +7416,25 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
-      <c r="I76" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="15"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
-      <c r="E77" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>170</v>
-      </c>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
       <c r="I77" s="3" t="s">
-        <v>253</v>
+        <v>149</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>171</v>
@@ -7331,23 +7443,19 @@
       <c r="L77" s="9"/>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="15"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
-      <c r="E78" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>170</v>
-      </c>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
       <c r="I78" s="3" t="s">
-        <v>148</v>
+        <v>252</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>171</v>
@@ -7356,15 +7464,15 @@
       <c r="L78" s="9"/>
     </row>
     <row r="79" spans="1:12">
-      <c r="A79" s="15"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>170</v>
@@ -7372,7 +7480,7 @@
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
       <c r="I79" s="3" t="s">
-        <v>142</v>
+        <v>253</v>
       </c>
       <c r="J79" s="3" t="s">
         <v>171</v>
@@ -7380,21 +7488,71 @@
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
     </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="18"/>
+      <c r="B80" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="18"/>
+      <c r="B81" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A48:A79"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A50:A81"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="G40:G41"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7406,7 +7564,7 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I43" sqref="A3:I43"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="14"/>
@@ -7425,19 +7583,19 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="15">
       <c r="A5" s="2" t="s">
@@ -7676,7 +7834,9 @@
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
@@ -7691,7 +7851,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -7699,7 +7859,9 @@
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>319</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
@@ -7714,13 +7876,15 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>320</v>
+      </c>
       <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
@@ -7735,13 +7899,15 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>321</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>33</v>
       </c>
@@ -7756,7 +7922,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
@@ -7775,10 +7941,10 @@
       <c r="F20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="3"/>
@@ -7800,8 +7966,8 @@
       <c r="F21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -8139,7 +8305,7 @@
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="18" t="s">
         <v>27</v>
       </c>
       <c r="H38" s="3"/>
@@ -8160,7 +8326,7 @@
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
@@ -8180,7 +8346,7 @@
         <v>12</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="18" t="s">
         <v>27</v>
       </c>
       <c r="I40" s="3"/>
@@ -8201,7 +8367,7 @@
         <v>12</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="15"/>
+      <c r="H41" s="18"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:10">
@@ -8258,22 +8424,22 @@
       <c r="J47" s="23"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="C48" s="15">
+      <c r="C48" s="18">
         <v>0</v>
       </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15">
+      <c r="D48" s="18"/>
+      <c r="E48" s="18">
         <v>1</v>
       </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15">
+      <c r="F48" s="18"/>
+      <c r="G48" s="18">
         <v>2</v>
       </c>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15">
+      <c r="H48" s="18"/>
+      <c r="I48" s="18">
         <v>3</v>
       </c>
-      <c r="J48" s="15"/>
+      <c r="J48" s="18"/>
     </row>
     <row r="49" spans="1:10">
       <c r="C49" s="3" t="s">
@@ -8302,7 +8468,7 @@
       </c>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="18" t="s">
         <v>175</v>
       </c>
       <c r="B50" s="3">
@@ -8334,7 +8500,7 @@
       </c>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="15"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="3">
         <f>B50+1</f>
         <v>1</v>
@@ -8365,7 +8531,7 @@
       </c>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="15"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="3">
         <f t="shared" ref="B52:B81" si="0">B51+1</f>
         <v>2</v>
@@ -8392,7 +8558,7 @@
       <c r="J52" s="9"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="15"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8419,7 +8585,7 @@
       <c r="J53" s="9"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="15"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8442,7 +8608,7 @@
       <c r="J54" s="9"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="15"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8465,7 +8631,7 @@
       <c r="J55" s="9"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="15"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8496,7 +8662,7 @@
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="15"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8523,7 +8689,7 @@
       </c>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="15"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8546,7 +8712,7 @@
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="15"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8569,7 +8735,7 @@
       </c>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="15"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8592,7 +8758,7 @@
       </c>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="15"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8615,7 +8781,7 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="15"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -8642,7 +8808,7 @@
       </c>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -8669,7 +8835,7 @@
       </c>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="15"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8688,7 +8854,7 @@
       </c>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8707,7 +8873,7 @@
       </c>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="15"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8730,7 +8896,7 @@
       <c r="J66" s="9"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="15"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8749,7 +8915,7 @@
       <c r="J67" s="9"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="15"/>
+      <c r="A68" s="18"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -8764,7 +8930,7 @@
       <c r="J68" s="9"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="15"/>
+      <c r="A69" s="18"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -8779,7 +8945,7 @@
       <c r="J69" s="9"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="15"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -8794,7 +8960,7 @@
       <c r="J70" s="9"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="15"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -8809,7 +8975,7 @@
       <c r="J71" s="9"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="15"/>
+      <c r="A72" s="18"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -8824,7 +8990,7 @@
       <c r="J72" s="9"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="15"/>
+      <c r="A73" s="18"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -8839,7 +9005,7 @@
       <c r="J73" s="9"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="15"/>
+      <c r="A74" s="18"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -8854,7 +9020,7 @@
       <c r="J74" s="9"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="15"/>
+      <c r="A75" s="18"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -8869,7 +9035,7 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="15"/>
+      <c r="A76" s="18"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -8884,7 +9050,7 @@
       <c r="J76" s="9"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="15"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -8903,7 +9069,7 @@
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="15"/>
+      <c r="A78" s="18"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -8922,7 +9088,7 @@
       </c>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="15"/>
+      <c r="A79" s="18"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -8945,7 +9111,7 @@
       </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="15"/>
+      <c r="A80" s="18"/>
       <c r="B80" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8968,7 +9134,7 @@
       </c>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="15"/>
+      <c r="A81" s="18"/>
       <c r="B81" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -9016,7 +9182,7 @@
   <dimension ref="B2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -9096,12 +9262,20 @@
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="11">
+        <v>45918</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="11">
+        <v>45920</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="11"/>
@@ -9166,6 +9340,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="43135f08-7c27-4a7c-bc6d-152a25501e39" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6946600b-d432-4ec1-a6de-e6a1f3354bfd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C98D15B0064474782E8EDBA35A51CC2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="84bc66ae19ca557e54d7014d86ef62c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6946600b-d432-4ec1-a6de-e6a1f3354bfd" xmlns:ns3="43135f08-7c27-4a7c-bc6d-152a25501e39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f294aa8e50c0a16a8ee0b06cd98abedc" ns2:_="" ns3:_="">
     <xsd:import namespace="6946600b-d432-4ec1-a6de-e6a1f3354bfd"/>
@@ -9372,7 +9557,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9381,18 +9566,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="43135f08-7c27-4a7c-bc6d-152a25501e39" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6946600b-d432-4ec1-a6de-e6a1f3354bfd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D7A352-4E74-4D3B-B371-7F84A478DD81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="43135f08-7c27-4a7c-bc6d-152a25501e39"/>
+    <ds:schemaRef ds:uri="6946600b-d432-4ec1-a6de-e6a1f3354bfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02F2913-AEC8-45FD-9F40-2703FA5F6AAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9411,21 +9596,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993051E6-CE55-49FB-9812-9A2B302725FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D7A352-4E74-4D3B-B371-7F84A478DD81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="43135f08-7c27-4a7c-bc6d-152a25501e39"/>
-    <ds:schemaRef ds:uri="6946600b-d432-4ec1-a6de-e6a1f3354bfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>